<commit_message>
Framework with License protection and pdf report
</commit_message>
<xml_diff>
--- a/FrameworkPOM/data/BCT.xlsx
+++ b/FrameworkPOM/data/BCT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="GridProperties" sheetId="3" r:id="rId3"/>
     <sheet name="MobileProperties" sheetId="4" r:id="rId4"/>
     <sheet name="ObjectRepository" sheetId="5" r:id="rId5"/>
+    <sheet name="MailProperties" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>UserName</t>
   </si>
@@ -204,6 +205,66 @@
   </si>
   <si>
     <t>Home.UserName.Xpath</t>
+  </si>
+  <si>
+    <t>AutomationType</t>
+  </si>
+  <si>
+    <t>Web Application</t>
+  </si>
+  <si>
+    <t>ApplicationName</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>HostName</t>
+  </si>
+  <si>
+    <t>PortName</t>
+  </si>
+  <si>
+    <t>SMPTauth</t>
+  </si>
+  <si>
+    <t>PassWord</t>
+  </si>
+  <si>
+    <t>FromAddress</t>
+  </si>
+  <si>
+    <t>ToAddress</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>pdfFileName</t>
+  </si>
+  <si>
+    <t>TestResultsReport.pdf</t>
+  </si>
+  <si>
+    <t>mail.bctchn.local</t>
+  </si>
+  <si>
+    <t>nijanthan.j@bahwancybertek.com</t>
+  </si>
+  <si>
+    <t>Test Execution Result in PDF</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -219,10 +280,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -254,6 +316,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -593,66 +656,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -822,122 +956,214 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="4" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>